<commit_message>
Split in Files with Renamed Columns
</commit_message>
<xml_diff>
--- a/data_impute_project/data/bird.xlsx
+++ b/data_impute_project/data/bird.xlsx
@@ -436,47 +436,47 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>species</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>specimen</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>habitat</t>
+          <t>C</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>diet</t>
+          <t>D</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>site</t>
+          <t>E</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>δ13C coll</t>
+          <t>F</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>δ15N coll</t>
+          <t>G</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>δ13C carb</t>
+          <t>H</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>δ18O carb</t>
+          <t>I</t>
         </is>
       </c>
     </row>

</xml_diff>